<commit_message>
Planned the test cases
Developed a test plan that covers the functions “sequentialSearch” and “binarySearch” .
</commit_message>
<xml_diff>
--- a/Amina_Aar_Test_Plan.xlsx
+++ b/Amina_Aar_Test_Plan.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nasro\Desktop\Final\JSAT2\part1And2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C66244FA-0968-481F-96ED-811196ACF349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180DE36E-BB81-4319-A9E7-6D07523DDA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{1CBCEDA5-E686-461F-8357-424248DC45AD}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" firstSheet="2" activeTab="3" xr2:uid="{1CBCEDA5-E686-461F-8357-424248DC45AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Test1 Binary Search Found Key" sheetId="1" r:id="rId1"/>
+    <sheet name="Test2 Binary Key Not Found" sheetId="3" r:id="rId2"/>
+    <sheet name="Test3 Linear KeyFound" sheetId="4" r:id="rId3"/>
+    <sheet name="Test 4 Linear Key Not Found" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -66,6 +69,107 @@
   </si>
   <si>
     <t>Pass / Fail / Not executed / Suspended</t>
+  </si>
+  <si>
+    <t>Check that the binarySearch() function correctly returns the index when the target number is found in the array</t>
+  </si>
+  <si>
+    <t>Amina Aar</t>
+  </si>
+  <si>
+    <t>Create sortedArray with sample values</t>
+  </si>
+  <si>
+    <t>Array is initialized correctly</t>
+  </si>
+  <si>
+    <t>Set key to 23</t>
+  </si>
+  <si>
+    <t>Target key is defined</t>
+  </si>
+  <si>
+    <t>Check result</t>
+  </si>
+  <si>
+    <t>Display result to console</t>
+  </si>
+  <si>
+    <t>Check that binarySearch() returns -1 when the target number is not in the array</t>
+  </si>
+  <si>
+    <t>create sortedArray with sample values</t>
+  </si>
+  <si>
+    <t>Array is initialised correctly</t>
+  </si>
+  <si>
+    <t>Call binarySearch( sortedArray, key)</t>
+  </si>
+  <si>
+    <t>Function executes without errors</t>
+  </si>
+  <si>
+    <t>Should return index 5( where 23 is located)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Result </t>
+  </si>
+  <si>
+    <t>Console shows "The key of 23 was found at index 5"</t>
+  </si>
+  <si>
+    <t>Set key to 83</t>
+  </si>
+  <si>
+    <t>Call binarySearch (sortedArray, key)</t>
+  </si>
+  <si>
+    <t>Should return -1 because 83 is not in the array</t>
+  </si>
+  <si>
+    <t>Console shows " The key of 83 was not found -1 "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that sequentialSearch() returns the correct index when the key exists in the array
+</t>
+  </si>
+  <si>
+    <t>Create searchArray with sample values</t>
+  </si>
+  <si>
+    <t>Set myKey to 25</t>
+  </si>
+  <si>
+    <t>Call sequentialSearch(searchArray, myKey)</t>
+  </si>
+  <si>
+    <t>Function executes without error</t>
+  </si>
+  <si>
+    <t>Should return index 4( where 25 is located)</t>
+  </si>
+  <si>
+    <t>Console shows "The key of 25 was found at index 4"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that sequentialSearch() returns -1 when the key does not exist in the array
+</t>
+  </si>
+  <si>
+    <t>Set myKey to 81</t>
+  </si>
+  <si>
+    <t>Call sequentialSearch(searchArray, mykey)</t>
+  </si>
+  <si>
+    <t>Function executes without errror</t>
+  </si>
+  <si>
+    <t>Should return -1 because 81 was not in the array</t>
+  </si>
+  <si>
+    <t>Console shows " The key of 81 was not found -1"</t>
   </si>
 </sst>
 </file>
@@ -646,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C4522D-3DA9-40EB-A4FE-33A63A4EB0A6}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -660,12 +764,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="C1" s="3">
+        <v>1</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2"/>
-      <c r="F1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -685,12 +793,14 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" ht="15.9">
+    <row r="3" spans="1:11" s="5" customFormat="1" ht="31.75">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
+      <c r="C3" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
@@ -745,9 +855,13 @@
       <c r="A7" s="20">
         <v>1</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="C7" s="21"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
@@ -760,7 +874,256 @@
       <c r="A8" s="20">
         <v>2</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" s="5" customFormat="1" ht="54.9" customHeight="1">
+      <c r="A9" s="20">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" s="5" customFormat="1" ht="55.75" customHeight="1">
+      <c r="A10" s="20">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" s="5" customFormat="1" ht="58.75" customHeight="1">
+      <c r="A11" s="20">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="F5:H6"/>
+    <mergeCell ref="I5:K6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1E460A-C27B-4EA5-8723-C15EAFD87BCD}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="30" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.9">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="31.75">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.9">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="15"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="38.15" customHeight="1">
+      <c r="A7" s="20">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.9">
+      <c r="A8" s="20">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="C8" s="25"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -771,13 +1134,17 @@
       <c r="J8" s="23"/>
       <c r="K8" s="24"/>
     </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" ht="31.75" customHeight="1">
+    <row r="9" spans="1:11" ht="40.299999999999997" customHeight="1">
       <c r="A9" s="20">
         <v>3</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C9" s="25"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="22"/>
       <c r="G9" s="23"/>
@@ -786,13 +1153,17 @@
       <c r="J9" s="27"/>
       <c r="K9" s="28"/>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" ht="32.6" customHeight="1">
+    <row r="10" spans="1:11" ht="48" customHeight="1">
       <c r="A10" s="20">
         <v>4</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="C10" s="25"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="22"/>
       <c r="G10" s="23"/>
@@ -801,13 +1172,522 @@
       <c r="J10" s="23"/>
       <c r="K10" s="24"/>
     </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" ht="32.6" customHeight="1">
+    <row r="11" spans="1:11" ht="45" customHeight="1">
       <c r="A11" s="20">
         <v>5</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" s="25"/>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="F5:H6"/>
+    <mergeCell ref="I5:K6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BF6FA7-7226-4354-A1DC-E6F5E27E8310}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <cols>
+    <col min="3" max="3" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="31.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.9">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="31.75">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.9">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="15"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="39" customHeight="1">
+      <c r="A7" s="20">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.9">
+      <c r="A8" s="20">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" ht="33.9" customHeight="1">
+      <c r="A9" s="20">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" ht="53.15" customHeight="1">
+      <c r="A10" s="20">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" ht="46.3" customHeight="1">
+      <c r="A11" s="20">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="F5:H6"/>
+    <mergeCell ref="I5:K6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E1FBB8A-410F-4525-B958-B1EC5400BAE9}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <cols>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="5" max="5" width="12.3046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="33" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.9">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.9">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.9">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="15"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="33" customHeight="1">
+      <c r="A7" s="20">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.9">
+      <c r="A8" s="20">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" ht="49.75" customHeight="1">
+      <c r="A9" s="20">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" ht="52.75" customHeight="1">
+      <c r="A10" s="20">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" ht="47.6" customHeight="1">
+      <c r="A11" s="20">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="22"/>
       <c r="G11" s="23"/>

</xml_diff>

<commit_message>
Coducted the test Cases
Conducted the tests in my test plan and recorded the results in  test plan file.
</commit_message>
<xml_diff>
--- a/Amina_Aar_Test_Plan.xlsx
+++ b/Amina_Aar_Test_Plan.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nasro\Desktop\Final\JSAT2\part1And2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C66244FA-0968-481F-96ED-811196ACF349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5AF08A-997B-4C12-861A-4B24DBC55D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{1CBCEDA5-E686-461F-8357-424248DC45AD}"/>
+    <workbookView xWindow="51" yWindow="4911" windowWidth="17280" windowHeight="9129" firstSheet="2" activeTab="3" xr2:uid="{1CBCEDA5-E686-461F-8357-424248DC45AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Test1 Binary Search Found Key" sheetId="1" r:id="rId1"/>
+    <sheet name="Test2 Binary Key Not Found" sheetId="3" r:id="rId2"/>
+    <sheet name="Test3 Linear KeyFound" sheetId="4" r:id="rId3"/>
+    <sheet name="Test 4 Linear Key Not Found" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -53,6 +56,9 @@
     <t>Test Result (Pass/Fail/Not Executed)</t>
   </si>
   <si>
+    <t>PASS</t>
+  </si>
+  <si>
     <t>Step #</t>
   </si>
   <si>
@@ -66,6 +72,158 @@
   </si>
   <si>
     <t>Pass / Fail / Not executed / Suspended</t>
+  </si>
+  <si>
+    <t>Check that the binarySearch() function correctly returns the index when the target number is found in the array</t>
+  </si>
+  <si>
+    <t>Amina Aar</t>
+  </si>
+  <si>
+    <t>Create sortedArray with sample values</t>
+  </si>
+  <si>
+    <t>Array is initialized correctly</t>
+  </si>
+  <si>
+    <t>Set key to 23</t>
+  </si>
+  <si>
+    <t>Target key is defined</t>
+  </si>
+  <si>
+    <t>Check result</t>
+  </si>
+  <si>
+    <t>Display result to console</t>
+  </si>
+  <si>
+    <t>Check that binarySearch() returns -1 when the target number is not in the array</t>
+  </si>
+  <si>
+    <t>create sortedArray with sample values</t>
+  </si>
+  <si>
+    <t>Array is initialised correctly</t>
+  </si>
+  <si>
+    <t>Call binarySearch( sortedArray, key)</t>
+  </si>
+  <si>
+    <t>Function executes without errors</t>
+  </si>
+  <si>
+    <t>Should return index 5( where 23 is located)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Result </t>
+  </si>
+  <si>
+    <t>Console shows "The key of 23 was found at index 5"</t>
+  </si>
+  <si>
+    <t>Set key to 83</t>
+  </si>
+  <si>
+    <t>Call binarySearch (sortedArray, key)</t>
+  </si>
+  <si>
+    <t>Should return -1 because 83 is not in the array</t>
+  </si>
+  <si>
+    <t>Console shows " The key of 83 was not found -1 "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that sequentialSearch() returns the correct index when the key exists in the array
+</t>
+  </si>
+  <si>
+    <t>Create searchArray with sample values</t>
+  </si>
+  <si>
+    <t>Set myKey to 25</t>
+  </si>
+  <si>
+    <t>Call sequentialSearch(searchArray, myKey)</t>
+  </si>
+  <si>
+    <t>Function executes without error</t>
+  </si>
+  <si>
+    <t>Should return index 4( where 25 is located)</t>
+  </si>
+  <si>
+    <t>Console shows "The key of 25 was found at index 4"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that sequentialSearch() returns -1 when the key does not exist in the array
+</t>
+  </si>
+  <si>
+    <t>Set myKey to 81</t>
+  </si>
+  <si>
+    <t>Call sequentialSearch(searchArray, mykey)</t>
+  </si>
+  <si>
+    <t>Function executes without errror</t>
+  </si>
+  <si>
+    <t>Should return -1 because 81 was not in the array</t>
+  </si>
+  <si>
+    <t>Console shows " The key of 81 was not found -1"</t>
+  </si>
+  <si>
+    <t>Array is initialised correctlY</t>
+  </si>
+  <si>
+    <t>[2,5,8,12,16,23, 38] created</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>key = 23</t>
+  </si>
+  <si>
+    <t>Ran successfully</t>
+  </si>
+  <si>
+    <t>Returned 5</t>
+  </si>
+  <si>
+    <t>Correct messaged logged</t>
+  </si>
+  <si>
+    <t>[2,5,8,12,16,23,38] created</t>
+  </si>
+  <si>
+    <t>key = 83</t>
+  </si>
+  <si>
+    <t>Returned -1</t>
+  </si>
+  <si>
+    <t>Correct message logged</t>
+  </si>
+  <si>
+    <t>[11, 5, 8, 25,16, 31] created</t>
+  </si>
+  <si>
+    <t>myKey = 25</t>
+  </si>
+  <si>
+    <t>Returned 4</t>
+  </si>
+  <si>
+    <t>[11, 5, 8, 3, 25, 16, 31] created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass </t>
+  </si>
+  <si>
+    <t>myKey = 81</t>
   </si>
 </sst>
 </file>
@@ -646,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C4522D-3DA9-40EB-A4FE-33A63A4EB0A6}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -660,12 +818,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="C1" s="3">
+        <v>1</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2"/>
-      <c r="F1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -685,45 +847,51 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" ht="15.9">
+    <row r="3" spans="1:11" s="5" customFormat="1" ht="31.75">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
+      <c r="C3" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="8"/>
-      <c r="F3" s="10"/>
+      <c r="F3" s="10">
+        <v>45828</v>
+      </c>
       <c r="G3" s="11"/>
       <c r="H3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="8"/>
-      <c r="J3" s="12"/>
+      <c r="J3" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="15.9"/>
     <row r="5" spans="1:11" s="5" customFormat="1" ht="15.9">
       <c r="A5" s="14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -745,14 +913,22 @@
       <c r="A7" s="20">
         <v>1</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C7" s="21"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="22"/>
+      <c r="F7" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G7" s="23"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="22"/>
+      <c r="I7" s="22" t="s">
+        <v>46</v>
+      </c>
       <c r="J7" s="23"/>
       <c r="K7" s="24"/>
     </row>
@@ -760,59 +936,913 @@
       <c r="A8" s="20">
         <v>2</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" s="5" customFormat="1" ht="54.9" customHeight="1">
+      <c r="A9" s="20">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" s="5" customFormat="1" ht="55.75" customHeight="1">
+      <c r="A10" s="20">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" s="5" customFormat="1" ht="58.75" customHeight="1">
+      <c r="A11" s="20">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="F5:H6"/>
+    <mergeCell ref="I5:K6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1E460A-C27B-4EA5-8723-C15EAFD87BCD}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="30" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.9">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="31.75">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="10">
+        <v>45828</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.9">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="15"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="38.15" customHeight="1">
+      <c r="A7" s="20">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.9">
+      <c r="A8" s="20">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C8" s="25"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="22"/>
+      <c r="F8" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="G8" s="23"/>
       <c r="H8" s="24"/>
-      <c r="I8" s="22"/>
+      <c r="I8" s="22" t="s">
+        <v>46</v>
+      </c>
       <c r="J8" s="23"/>
       <c r="K8" s="24"/>
     </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" ht="31.75" customHeight="1">
+    <row r="9" spans="1:11" ht="40.299999999999997" customHeight="1">
       <c r="A9" s="20">
         <v>3</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="C9" s="25"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="22"/>
+      <c r="F9" s="22" t="s">
+        <v>48</v>
+      </c>
       <c r="G9" s="23"/>
       <c r="H9" s="24"/>
-      <c r="I9" s="26"/>
+      <c r="I9" s="26" t="s">
+        <v>46</v>
+      </c>
       <c r="J9" s="27"/>
       <c r="K9" s="28"/>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" ht="32.6" customHeight="1">
+    <row r="10" spans="1:11" ht="48" customHeight="1">
       <c r="A10" s="20">
         <v>4</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="C10" s="25"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="22"/>
+      <c r="F10" s="22" t="s">
+        <v>53</v>
+      </c>
       <c r="G10" s="23"/>
       <c r="H10" s="24"/>
-      <c r="I10" s="22"/>
+      <c r="I10" s="22" t="s">
+        <v>46</v>
+      </c>
       <c r="J10" s="23"/>
       <c r="K10" s="24"/>
     </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" ht="32.6" customHeight="1">
+    <row r="11" spans="1:11" ht="45" customHeight="1">
       <c r="A11" s="20">
         <v>5</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="C11" s="25"/>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="22"/>
+      <c r="F11" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="G11" s="23"/>
       <c r="H11" s="24"/>
-      <c r="I11" s="22"/>
+      <c r="I11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="F5:H6"/>
+    <mergeCell ref="I5:K6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BF6FA7-7226-4354-A1DC-E6F5E27E8310}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <cols>
+    <col min="3" max="3" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="31.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.9">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.9">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="10">
+        <v>45828</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.9">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="15"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="39" customHeight="1">
+      <c r="A7" s="20">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.9">
+      <c r="A8" s="20">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" ht="33.9" customHeight="1">
+      <c r="A9" s="20">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" ht="53.15" customHeight="1">
+      <c r="A10" s="20">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" ht="46.3" customHeight="1">
+      <c r="A11" s="20">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="F5:H6"/>
+    <mergeCell ref="I5:K6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E1FBB8A-410F-4525-B958-B1EC5400BAE9}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <cols>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="5" max="5" width="12.3046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="33" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.9">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.9">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="10">
+        <v>45828</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.9">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="15"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="33" customHeight="1">
+      <c r="A7" s="20">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.9">
+      <c r="A8" s="20">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" ht="49.75" customHeight="1">
+      <c r="A9" s="20">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" ht="52.75" customHeight="1">
+      <c r="A10" s="20">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" ht="47.6" customHeight="1">
+      <c r="A11" s="20">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="22" t="s">
+        <v>46</v>
+      </c>
       <c r="J11" s="23"/>
       <c r="K11" s="24"/>
     </row>

</xml_diff>